<commit_message>
Added alternate jobs plot.
</commit_message>
<xml_diff>
--- a/library/Generic_facilities.xlsx
+++ b/library/Generic_facilities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060AD4A9-5A56-46AC-A294-141160DBABD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD3EE6-607E-440B-91AA-CE1ACFD27338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="28680" yWindow="-1065" windowWidth="29040" windowHeight="15840" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,10 @@
     <sheet name="Array cable" sheetId="7" r:id="rId5"/>
     <sheet name="Export cable" sheetId="4" r:id="rId6"/>
     <sheet name="Monopile" sheetId="1" r:id="rId7"/>
-    <sheet name="WTIV" sheetId="8" r:id="rId8"/>
+    <sheet name="Jacket" sheetId="9" r:id="rId8"/>
+    <sheet name="Semisubmersible" sheetId="11" r:id="rId9"/>
+    <sheet name="Offshore substation" sheetId="10" r:id="rId10"/>
+    <sheet name="WTIV" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="51">
   <si>
     <t>Factory specifications</t>
   </si>
@@ -174,13 +177,34 @@
   </si>
   <si>
     <t>WTIV 3</t>
+  </si>
+  <si>
+    <t>jackets/year</t>
+  </si>
+  <si>
+    <t>Jacket 1</t>
+  </si>
+  <si>
+    <t>substation/year</t>
+  </si>
+  <si>
+    <t>semisubs/year</t>
+  </si>
+  <si>
+    <t>Semisubmersible 1</t>
+  </si>
+  <si>
+    <t>Semisubmersible 3</t>
+  </si>
+  <si>
+    <t>Semisubmersible 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +229,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,15 +579,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF66AA12-E0D8-42F1-83CD-A592BFF5EB2C}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -665,6 +695,383 @@
       </c>
       <c r="B13">
         <v>2026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17">
+        <v>2030</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B0B918-E104-4E21-9FCD-E0D518BA7C95}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>100</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>7.1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>2.4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4.7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>100-SUM(B14:B16)-B18</f>
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>11.8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2516E4F7-AB48-42A0-9912-12CC392793F4}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>466</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1407,8 +1814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ACB539-34F9-4F03-9718-22E78997971A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1574,18 +1981,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2516E4F7-AB48-42A0-9912-12CC392793F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8413F004-DA56-47B2-9CA5-F34D53B4E73F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1604,10 +2010,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1615,7 +2021,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1667,7 +2073,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>466</v>
+        <v>425</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1678,7 +2084,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -1689,7 +2095,7 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>20</v>
+        <v>7.1</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1700,7 +2106,7 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>2.4</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -1711,7 +2117,7 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>20</v>
+        <v>4.7</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -1722,7 +2128,8 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>30</v>
+        <f>100-SUM(B14:B16)-B18</f>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -1733,7 +2140,160 @@
         <v>19</v>
       </c>
       <c r="B18">
+        <v>11.8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA885459-4D29-4DEE-9AD2-5F444EBA6123}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Adding additional plot scripts for direct/indirect jobs
</commit_message>
<xml_diff>
--- a/library/Generic_facilities.xlsx
+++ b/library/Generic_facilities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8753D1AC-E69C-4BE9-B909-6216A40DA257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D700583D-D877-4A3C-BF37-14A2D6F717ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="11" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="3" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="60">
   <si>
     <t>Factory specifications</t>
   </si>
@@ -205,6 +205,27 @@
   </si>
   <si>
     <t>Steel plate 1</t>
+  </si>
+  <si>
+    <t>Notes and assumptions</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Keppel Amfels (Begin construction right after Charybdis)</t>
+  </si>
+  <si>
+    <t>Philly shipyard (Clear order books in 2025)</t>
+  </si>
+  <si>
+    <t>VT Halter (Clear order books in 2025)</t>
   </si>
 </sst>
 </file>
@@ -586,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF66AA12-E0D8-42F1-83CD-A592BFF5EB2C}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +618,7 @@
     <col min="1" max="1" width="19.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -607,8 +628,11 @@
       <c r="C1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -616,7 +640,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -624,7 +648,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -632,7 +656,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -640,7 +664,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -648,7 +672,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -656,7 +680,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -664,7 +688,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -672,7 +696,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -680,31 +704,49 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
       <c r="B11">
         <v>2026</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>42</v>
       </c>
       <c r="B12">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2028</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>43</v>
       </c>
       <c r="B13">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+        <v>2028</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -712,7 +754,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -720,7 +762,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1098,7 +1140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3BDA63-043F-4F6F-AF7D-07E7E696E20C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated scenarios to match demand better
</commit_message>
<xml_diff>
--- a/library/Generic_facilities.xlsx
+++ b/library/Generic_facilities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E159DA2-3C5B-448F-ACE0-241886607C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2971DB-8804-4BE3-98CB-A63F24714CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>Array cable 1</t>
   </si>
   <si>
-    <t>Array cable 2</t>
-  </si>
-  <si>
     <t>Blade 3</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Transition piece 1</t>
+  </si>
+  <si>
+    <t>Tower 2</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,7 +633,7 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -654,7 +654,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>2026</v>
@@ -678,15 +678,15 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B7">
-        <v>2028</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>2028</v>
@@ -710,49 +710,49 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>2026</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>2028</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>2028</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14">
         <v>2024</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>2028</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <v>2029</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17">
         <v>2030</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>2028</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>2025</v>
@@ -838,7 +838,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1335,7 +1335,7 @@
         <v>120000</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2577,7 +2577,7 @@
         <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added GBF to port screen and roadmap results.  Added bedplate and flange to port screen
</commit_message>
<xml_diff>
--- a/library/Generic_facilities.xlsx
+++ b/library/Generic_facilities.xlsx
@@ -8,30 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344401F2-51FB-40F3-86F0-EEF34728BB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE7B43F-F1D1-4DA0-A400-354C8F6810DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Avg Demand Scenario" sheetId="3" r:id="rId1"/>
-    <sheet name="Blade" sheetId="2" r:id="rId2"/>
-    <sheet name="Nacelle" sheetId="5" r:id="rId3"/>
-    <sheet name="Tower" sheetId="6" r:id="rId4"/>
-    <sheet name="Array cable" sheetId="7" r:id="rId5"/>
-    <sheet name="Export cable" sheetId="4" r:id="rId6"/>
-    <sheet name="Monopile" sheetId="1" r:id="rId7"/>
-    <sheet name="Transition piece" sheetId="13" r:id="rId8"/>
-    <sheet name="Jacket" sheetId="9" r:id="rId9"/>
-    <sheet name="Semisubmersible" sheetId="11" r:id="rId10"/>
-    <sheet name="Offshore substation" sheetId="10" r:id="rId11"/>
-    <sheet name="WTIV" sheetId="8" r:id="rId12"/>
-    <sheet name="Steel plate" sheetId="12" r:id="rId13"/>
-    <sheet name="Flange" sheetId="14" r:id="rId14"/>
+    <sheet name="Mooring chain" sheetId="15" r:id="rId2"/>
+    <sheet name="Mooring rope" sheetId="16" r:id="rId3"/>
+    <sheet name="Blade" sheetId="2" r:id="rId4"/>
+    <sheet name="Nacelle" sheetId="5" r:id="rId5"/>
+    <sheet name="Tower" sheetId="6" r:id="rId6"/>
+    <sheet name="Array cable" sheetId="7" r:id="rId7"/>
+    <sheet name="Export cable" sheetId="4" r:id="rId8"/>
+    <sheet name="Monopile" sheetId="1" r:id="rId9"/>
+    <sheet name="Transition piece" sheetId="13" r:id="rId10"/>
+    <sheet name="Jacket" sheetId="9" r:id="rId11"/>
+    <sheet name="Semisubmersible" sheetId="11" r:id="rId12"/>
+    <sheet name="GBF" sheetId="17" r:id="rId13"/>
+    <sheet name="Offshore substation" sheetId="10" r:id="rId14"/>
+    <sheet name="WTIV" sheetId="8" r:id="rId15"/>
+    <sheet name="Steel plate" sheetId="12" r:id="rId16"/>
+    <sheet name="Flange" sheetId="14" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="79">
   <si>
     <t>Factory specifications</t>
   </si>
@@ -249,6 +253,45 @@
   </si>
   <si>
     <t>#/year</t>
+  </si>
+  <si>
+    <t>Blade 4</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Nacelle 2</t>
+  </si>
+  <si>
+    <t>Tower 3</t>
+  </si>
+  <si>
+    <t>Mooring chain 1</t>
+  </si>
+  <si>
+    <t>Mooring rope 1</t>
+  </si>
+  <si>
+    <t>(excluding port development costs)</t>
+  </si>
+  <si>
+    <t>(from announcement to full operational status)</t>
+  </si>
+  <si>
+    <t>Semisubmersible 1</t>
+  </si>
+  <si>
+    <t>GBF/year</t>
+  </si>
+  <si>
+    <t>Equipment and some facility upgrades</t>
+  </si>
+  <si>
+    <t>Rough average of RCAM and Esteyco</t>
+  </si>
+  <si>
+    <t>GBF 1</t>
   </si>
 </sst>
 </file>
@@ -374,7 +417,40 @@
       <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9" refreshError="1"/>
       <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1">
+        <row r="44">
+          <cell r="S44">
+            <v>1</v>
+          </cell>
+          <cell r="AW44">
+            <v>2000</v>
+          </cell>
+          <cell r="AX44">
+            <v>50</v>
+          </cell>
+          <cell r="AY44">
+            <v>2</v>
+          </cell>
+          <cell r="BK44">
+            <v>100</v>
+          </cell>
+          <cell r="BL44">
+            <v>0.05</v>
+          </cell>
+          <cell r="BM44">
+            <v>0.1</v>
+          </cell>
+          <cell r="BN44">
+            <v>0.05</v>
+          </cell>
+          <cell r="BO44">
+            <v>0.75</v>
+          </cell>
+          <cell r="BP44">
+            <v>0.05</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="12" refreshError="1"/>
       <sheetData sheetId="13" refreshError="1"/>
       <sheetData sheetId="14" refreshError="1"/>
@@ -709,19 +785,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF66AA12-E0D8-42F1-83CD-A592BFF5EB2C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -735,7 +811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -746,7 +822,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -757,7 +833,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -768,7 +844,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -779,7 +855,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -790,7 +866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -801,7 +877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -812,7 +888,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -823,7 +899,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -834,7 +910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -845,7 +921,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -856,61 +932,138 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>47</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>2029</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>50</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>2025</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>2026</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>2028</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>2029</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>64</v>
+      </c>
+      <c r="B19">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20">
+        <v>2030</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <v>2030</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22">
+        <v>2030</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23">
+        <v>2030</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24">
+        <v>2030</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>2030</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -921,6 +1074,348 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B190784-80A5-46FF-B5D5-B70F3B4F7CDA}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8413F004-DA56-47B2-9CA5-F34D53B4E73F}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>425</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>7.1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>2.4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>4.7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>100-SUM(B14:B16)-B18</f>
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>11.8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA885459-4D29-4DEE-9AD2-5F444EBA6123}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -928,14 +1423,14 @@
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +1441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -957,7 +1452,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -968,7 +1463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -979,37 +1474,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1020,7 +1515,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1028,7 +1523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1036,7 +1531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1044,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1052,7 +1547,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1555,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1073,7 +1568,118 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7839A3-CCAE-465E-BDC4-042D07C23AB8}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>350</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B0B918-E104-4E21-9FCD-E0D518BA7C95}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1081,14 +1687,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1110,7 +1716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1121,7 +1727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1132,37 +1738,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1184,7 +1790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1801,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1217,7 +1823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1229,7 +1835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2516E4F7-AB48-42A0-9912-12CC392793F4}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1254,14 +1860,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,7 +1878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1283,7 +1889,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1294,7 +1900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1305,37 +1911,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1952,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1357,7 +1963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1368,7 +1974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1985,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1390,7 +1996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1401,7 +2007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1417,7 +2023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3BDA63-043F-4F6F-AF7D-07E7E696E20C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1425,14 +2031,14 @@
       <selection sqref="A1:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="19.6328125" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1443,7 +2049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1454,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1465,7 +2071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1476,37 +2082,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1517,7 +2123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1528,7 +2134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1539,7 +2145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1550,7 +2156,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +2167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1572,7 +2178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1588,7 +2194,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF6D9F9-42CE-4C05-817C-410AD5AB0AEA}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -1596,14 +2202,14 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +2220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1625,7 +2231,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1636,7 +2242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1647,37 +2253,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1689,7 +2295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1698,7 +2304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1710,7 +2316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1722,7 +2328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1734,7 +2340,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1746,7 +2352,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1764,21 +2370,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E394EF1B-23F5-4178-BDD5-DE2DF9A8BA3C}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CE2D8A-502E-40E6-83C7-E6FA45CCA6CC}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1789,116 +2390,129 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>275</v>
+        <f>'[1]Mooring chain'!$AW$44</f>
+        <v>2000</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3">
-        <v>250</v>
+        <f>'[1]Mooring chain'!$AX$44</f>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
       <c r="B4">
-        <v>3.5</v>
+        <f>'[1]Mooring chain'!$AY$44</f>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>520</v>
+        <f>'[1]Mooring chain'!$BK$44</f>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>20</v>
+      <c r="B8" s="4">
+        <f>'[1]Mooring chain'!$BL$44</f>
+        <v>0.05</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>15</v>
+      <c r="B9" s="4">
+        <f>'[1]Mooring chain'!$BM$44</f>
+        <v>0.1</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
-        <v>20</v>
+      <c r="B10" s="4">
+        <f>'[1]Mooring chain'!$BN$44</f>
+        <v>0.05</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>30</v>
+      <c r="B11" s="4">
+        <f>'[1]Mooring chain'!$BO$44</f>
+        <v>0.75</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12">
-        <v>5</v>
+      <c r="B12" s="4">
+        <f>'[1]Mooring chain'!$BP$44</f>
+        <v>0.05</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -1910,6 +2524,306 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB031929-1311-4696-8843-DEF1936FC85F}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>'[1]Mooring chain'!$AW$44</f>
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>'[1]Mooring chain'!$AX$44</f>
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <f>'[1]Mooring chain'!$AY$44</f>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <f>'[1]Mooring chain'!$BK$44</f>
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4">
+        <f>'[1]Mooring chain'!$BL$44</f>
+        <v>0.05</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <f>'[1]Mooring chain'!$BM$44</f>
+        <v>0.1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="4">
+        <f>'[1]Mooring chain'!$BN$44</f>
+        <v>0.05</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4">
+        <f>'[1]Mooring chain'!$BO$44</f>
+        <v>0.75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4">
+        <f>'[1]Mooring chain'!$BP$44</f>
+        <v>0.05</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E394EF1B-23F5-4178-BDD5-DE2DF9A8BA3C}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>275</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>250</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>520</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E85467-6043-4D69-B0A9-8F782553D9FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -1917,14 +2831,14 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +2849,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1946,7 +2860,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1957,7 +2871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1968,12 +2882,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1984,7 +2898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1995,7 +2909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2006,7 +2920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2017,7 +2931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2028,7 +2942,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2039,7 +2953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2056,7 +2970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7784707C-9E6D-44AC-8547-8A58A3185976}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -2064,14 +2978,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2082,7 +2996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2093,7 +3007,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2104,7 +3018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2115,12 +3029,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2131,7 +3045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2142,7 +3056,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2153,7 +3067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2164,7 +3078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2175,7 +3089,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2186,7 +3100,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2202,7 +3116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A72919-2B5A-4AFC-B28B-5ED69A74E01A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -2210,14 +3124,14 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +3142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2239,7 +3153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2250,7 +3164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2261,12 +3175,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2277,7 +3191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2288,7 +3202,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2299,7 +3213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2310,7 +3224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2321,7 +3235,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2332,7 +3246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2348,7 +3262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7000F0EB-6A67-446D-9FE1-E6B7CE544415}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -2356,14 +3270,14 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2374,7 +3288,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2385,7 +3299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2396,7 +3310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2407,12 +3321,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2423,7 +3337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2434,7 +3348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2445,7 +3359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2456,7 +3370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2467,7 +3381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2478,7 +3392,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2494,7 +3408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ACB539-34F9-4F03-9718-22E78997971A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -2502,13 +3416,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2519,7 +3433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2530,7 +3444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2541,7 +3455,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2552,37 +3466,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2593,7 +3507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2604,7 +3518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2615,7 +3529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2626,7 +3540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2637,7 +3551,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2648,354 +3562,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
         <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B190784-80A5-46FF-B5D5-B70F3B4F7CDA}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>2.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>30</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8413F004-DA56-47B2-9CA5-F34D53B4E73F}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>3.5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>425</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>7.1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>2.4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>4.7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <f>100-SUM(B14:B16)-B18</f>
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>11.8</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Add port scenario spreadsheets with min and max facility development timelines
</commit_message>
<xml_diff>
--- a/library/Generic_facilities.xlsx
+++ b/library/Generic_facilities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\Analysis repos\Roadmap\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F240E0D-ADA4-4351-BA20-373BB965269E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5213601-BDE4-4249-8987-E753DD471D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2960" yWindow="2840" windowWidth="14400" windowHeight="7360" activeTab="3" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="11" xr2:uid="{6E624DB9-F13A-4642-BD3E-921B94A6B6A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mooring chain" sheetId="15" r:id="rId1"/>
@@ -1049,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8413F004-DA56-47B2-9CA5-F34D53B4E73F}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1086,7 +1086,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -1097,7 +1097,7 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -2578,7 +2578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E85467-6043-4D69-B0A9-8F782553D9FF}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>